<commit_message>
Updated GitIgnore and adding colour coding
For the belbin template, because I keep on having trouble looking between the two
</commit_message>
<xml_diff>
--- a/Belbin Template.xlsx
+++ b/Belbin Template.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisydneyedu-my.sharepoint.com/personal/rgup6136_uni_sydney_edu_au/Documents/2018 - S2/ENGG4111/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\PersonalityQuestionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CEA8DB1-D232-4E45-A6BE-629C6974631E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92D9093-ACD7-444C-AA1D-767FA00C996B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" activeTab="1" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table" sheetId="1" r:id="rId1"/>
+    <sheet name="S2" sheetId="4" r:id="rId2"/>
+    <sheet name="S3" sheetId="3" r:id="rId3"/>
+    <sheet name="S4" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Section</t>
   </si>
@@ -79,13 +82,94 @@
   </si>
   <si>
     <t>CF</t>
+  </si>
+  <si>
+    <t>Section 4. My characteristic approach to group work is that:</t>
+  </si>
+  <si>
+    <t>(a)I have a quiet interest in getting to know colleagues better.</t>
+  </si>
+  <si>
+    <t>(b)I am not reluctant to challenge the views of others or to hold a minority view myself.</t>
+  </si>
+  <si>
+    <t>(c)I can usually find a line of argument to refute unsound propositions.</t>
+  </si>
+  <si>
+    <t>(d)I think I have a talent for making things work once a plan has to be put into operation.</t>
+  </si>
+  <si>
+    <t>(e)I have a tendency to avoid the obvious and to come out with the unexpected.</t>
+  </si>
+  <si>
+    <t>(f) I bring a touch of perfectionism to any team job I undertake.</t>
+  </si>
+  <si>
+    <t>(g)I am ready to make use of contacts outside the group itself.</t>
+  </si>
+  <si>
+    <t>Section 3. When involved in a project with other people:</t>
+  </si>
+  <si>
+    <t>(a)I have an aptitude for influencing people without pressurizing them.</t>
+  </si>
+  <si>
+    <t>(b)My general vigilance percents careless mistakes and omissions being made.</t>
+  </si>
+  <si>
+    <t>(d)I can be counted on to contribute something original.</t>
+  </si>
+  <si>
+    <t>(e)I am always ready to back a good suggestion in the common interest.</t>
+  </si>
+  <si>
+    <t>(f) I am keen to look for the latest in new ideas and developments.</t>
+  </si>
+  <si>
+    <t>(g)I believe my capacity for cool judgments is appreciated by others.</t>
+  </si>
+  <si>
+    <t>(h)I can be relied upon to see that all essential work is organized.</t>
+  </si>
+  <si>
+    <t>Section 2. If I have a possible shortcoming in teamwork, it could be that:</t>
+  </si>
+  <si>
+    <t>(a)I am not at ease unless meetings are well structured and controlled and generally well conducted.</t>
+  </si>
+  <si>
+    <t>(c)I have a tendency to talk a lot once the group gets on to new ideas.</t>
+  </si>
+  <si>
+    <t>(d)My objective outlook makes it difficult for me to join in readily and enthusiastically with colleagues.</t>
+  </si>
+  <si>
+    <t>(e)I am sometimes seen as forceful and authoritarian if there is a need to get something done.</t>
+  </si>
+  <si>
+    <t>(f) I find it difficult to lead from the front, perhaps because I am over-responsive to group atmosphere.</t>
+  </si>
+  <si>
+    <t>(g)I am apt to get too caught up in ideas that occur to me and so lose track of what is happening.</t>
+  </si>
+  <si>
+    <t>(c)I am ready to press for action to make sure that the meeting does not waste  time or lose sight of the main objective.</t>
+  </si>
+  <si>
+    <t>(h)My colleagues tend to see me as worrying unnecessarily over detail and the possibility that things may go wrong.</t>
+  </si>
+  <si>
+    <t>(b)I am inclined to be too generous towards others who have a valid viewpoint that has not been given a proper airing.</t>
+  </si>
+  <si>
+    <t>(h)While I am interested in all views, I have no hesitation in making up my mind once a decision has to be made.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +183,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial-BoldMT"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="ArialMT"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -135,6 +230,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,16 +548,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1B4296-D68F-40AA-A935-AFB247084132}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,43 +589,118 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
         <f>SUM(B2:I2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2">
         <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J8" si="0">SUM(B3:I3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2">
         <v>4</v>
       </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -537,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -546,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -555,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,13 +756,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12" s="2">
         <v>1</v>
       </c>
       <c r="B12">
         <f>H2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <f>E2</f>
@@ -598,36 +770,36 @@
       </c>
       <c r="D12">
         <f>G2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <f>D2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <f>B2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f>I2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f>C2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f>F2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13">
         <f>B3</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <f>C3</f>
@@ -635,15 +807,15 @@
       </c>
       <c r="D13">
         <f>F3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f>H3</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <f>D3</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13">
         <f>E3</f>
@@ -655,20 +827,20 @@
       </c>
       <c r="I13">
         <f>I3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="2">
         <v>3</v>
       </c>
       <c r="B14">
         <f>I4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <f>B4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <f>D4</f>
@@ -676,11 +848,11 @@
       </c>
       <c r="E14">
         <f>E4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <f>G4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14">
         <f>H4</f>
@@ -688,14 +860,14 @@
       </c>
       <c r="H14">
         <f>F4</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I14">
         <f>C4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -705,7 +877,7 @@
       </c>
       <c r="C15">
         <f>I5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <f>C5</f>
@@ -717,7 +889,7 @@
       </c>
       <c r="F15">
         <f>H5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <f>D5</f>
@@ -729,10 +901,10 @@
       </c>
       <c r="I15">
         <f>G5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="2">
         <v>5</v>
       </c>
@@ -769,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -806,7 +978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>7</v>
       </c>
@@ -843,44 +1015,279 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19">
         <f>SUM(B12:B18)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:I19" si="1">SUM(C12:C18)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA1E97E-A678-4D10-A8E9-2742BC8C75D4}">
+  <dimension ref="B4:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4" spans="2:2">
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABE5DF9-E7E6-4E82-9836-F1BB36BDE3D7}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F96EB0-2018-48EE-97B6-0E76930E5B6D}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added colour coding to belbin workbook
</commit_message>
<xml_diff>
--- a/Belbin Template.xlsx
+++ b/Belbin Template.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\PersonalityQuestionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92D9093-ACD7-444C-AA1D-767FA00C996B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C0A91-DC52-4581-9721-3E1CEAF061C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" activeTab="1" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" activeTab="5" xr2:uid="{E0209042-E664-4103-A5FE-D1E5EFD81B12}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
-    <sheet name="S2" sheetId="4" r:id="rId2"/>
-    <sheet name="S3" sheetId="3" r:id="rId3"/>
-    <sheet name="S4" sheetId="2" r:id="rId4"/>
+    <sheet name="S1" sheetId="8" r:id="rId2"/>
+    <sheet name="S2" sheetId="4" r:id="rId3"/>
+    <sheet name="S3" sheetId="3" r:id="rId4"/>
+    <sheet name="S4" sheetId="2" r:id="rId5"/>
+    <sheet name="S5" sheetId="5" r:id="rId6"/>
+    <sheet name="S6" sheetId="6" r:id="rId7"/>
+    <sheet name="S7" sheetId="7" r:id="rId8"/>
+    <sheet name="References" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
   <si>
     <t>Section</t>
   </si>
@@ -163,13 +169,124 @@
   </si>
   <si>
     <t>(h)While I am interested in all views, I have no hesitation in making up my mind once a decision has to be made.</t>
+  </si>
+  <si>
+    <t>Section 5. I gain satisfaction in a job because:</t>
+  </si>
+  <si>
+    <t>(a)I enjoy analyzing situations and weighing up all the possible choices.</t>
+  </si>
+  <si>
+    <t>(b)I am interested in finding practical solutions to problems.</t>
+  </si>
+  <si>
+    <t>(c)I like to feel I am fostering good working relationships.</t>
+  </si>
+  <si>
+    <t>(d)I can have a strong influence on decisions.</t>
+  </si>
+  <si>
+    <t>(e)I can meet people who may have something new to offer.</t>
+  </si>
+  <si>
+    <t>(f) I can get people to agree on a necessary course of action.</t>
+  </si>
+  <si>
+    <t>(g)I feel in my element where I can give a task my full attention.</t>
+  </si>
+  <si>
+    <t>(h)I like to find a field that stretches my imagination.</t>
+  </si>
+  <si>
+    <t>Section 6. If I am suddenly given a difficult task with limited time and unfamiliar people:</t>
+  </si>
+  <si>
+    <t>(a)I would feel like retiring to a corner to devise a way out of the impasse before developing a line.</t>
+  </si>
+  <si>
+    <t>(b)I would be ready to work with the person who showed the most positive approach, however difficult he/she might be.</t>
+  </si>
+  <si>
+    <t>(d)My natural sense of urgency would help to ensure that we did not fall behind schedule.</t>
+  </si>
+  <si>
+    <t>(e)I believe I would keep cool and maintain my capacity to think straight.</t>
+  </si>
+  <si>
+    <t>(f) I would retain a steadiness of purpose in spite of the pressures.</t>
+  </si>
+  <si>
+    <t>(g)I would be prepared to take a positive lead it I felt the group was making no progress.</t>
+  </si>
+  <si>
+    <t>(h)I would open up discussion with a view to stimulating new thoughts and getting something moving.</t>
+  </si>
+  <si>
+    <t>(c)I would find some way of reducing the size of the task by establishing what different individuals might best contribute.</t>
+  </si>
+  <si>
+    <t>Section 7. With reference to the problems to which I am subject in working in groups:</t>
+  </si>
+  <si>
+    <t>(a)I am apt to show my impatience with those who are obstructing progress.</t>
+  </si>
+  <si>
+    <t>(b)Others may criticize me for being too analytical and insufficiently intuitive.</t>
+  </si>
+  <si>
+    <t>(c)My desire to ensure that work is properly done can hold up proceedings.</t>
+  </si>
+  <si>
+    <t>(d)I tend to get bored rather easily and rely on 1 or 2 stimulating people to spark me off.</t>
+  </si>
+  <si>
+    <t>(e)I find it difficult to get started unless the goals are clear.</t>
+  </si>
+  <si>
+    <t>(f) I am sometimes poor at explaining and clarifying complex points that occur to me.</t>
+  </si>
+  <si>
+    <t>(g)I a conscious of demanding from others the things I cannot do myself.</t>
+  </si>
+  <si>
+    <t>(h)I hesitate to get my points across when I run up against real opposition.</t>
+  </si>
+  <si>
+    <t>REF: R. Meredith Belbin, Management Teams: Why They Succeed or Fail, Butterworth-Heinemann, Jordan Hill, Oxford, 1993</t>
+  </si>
+  <si>
+    <t>Section 1 What I believe I can contribute to a team:</t>
+  </si>
+  <si>
+    <t>(a)I think I can quickly see and take advantage of new opportunities.</t>
+  </si>
+  <si>
+    <t>(b)I can work well with a very wide range of people.</t>
+  </si>
+  <si>
+    <t>(c)Producing ideas is one of my natural assets.</t>
+  </si>
+  <si>
+    <t>(e)My capacity to follow through has much to do with my personal effectiveness.</t>
+  </si>
+  <si>
+    <t>(f) I am ready to face temporary unpopularity if it leads to worthwhile results in the end.</t>
+  </si>
+  <si>
+    <t>(g)I am quick to sense what is likely to work in a situation with which I am familiar.</t>
+  </si>
+  <si>
+    <t>(h)I can offer a reasoned case for alternative courses of action without introducing bias or prejudice.</t>
+  </si>
+  <si>
+    <t>(d)My ability rests in being able to draw people out whenever I detect they have something of value to contribute to group objectives.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,8 +312,13 @@
       <color rgb="FF000000"/>
       <name val="ArialMT"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="ArialMT"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +328,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,14 +400,58 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FFFFFF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -548,9 +762,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1B4296-D68F-40AA-A935-AFB247084132}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -561,25 +776,25 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -593,22 +808,23 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
+      <c r="B2" s="23">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="26">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
         <v>2</v>
       </c>
       <c r="I2">
@@ -623,22 +839,23 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="23">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="7">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+      <c r="F3" s="26">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
         <v>3</v>
       </c>
       <c r="I3">
@@ -653,25 +870,25 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
+      <c r="B4" s="23">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2</v>
+      </c>
+      <c r="F4" s="26">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="13">
         <v>0</v>
       </c>
       <c r="I4">
@@ -686,24 +903,44 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
+      <c r="B5" s="23">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="2">
         <v>5</v>
       </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="13"/>
       <c r="J6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -713,6 +950,13 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="13"/>
       <c r="J7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -722,6 +966,13 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="13"/>
       <c r="J8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -873,11 +1124,11 @@
       </c>
       <c r="B15">
         <f>E5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <f>I5</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <f>C5</f>
@@ -885,7 +1136,7 @@
       </c>
       <c r="E15">
         <f>F5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <f>H5</f>
@@ -893,15 +1144,15 @@
       </c>
       <c r="G15">
         <f>D5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <f>B5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <f>G5</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1021,11 +1272,11 @@
       </c>
       <c r="B19">
         <f>SUM(B12:B18)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:I19" si="1">SUM(C12:C18)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
@@ -1033,7 +1284,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
@@ -1041,15 +1292,15 @@
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1058,62 +1309,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA1E97E-A678-4D10-A8E9-2742BC8C75D4}">
-  <dimension ref="B4:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0040741-549C-4C0A-B9F2-8D7E11F2B3CC}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="125.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:2">
-      <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2">
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2">
-      <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2">
-      <c r="B14" s="4"/>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="25" customFormat="1">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="25" customFormat="1">
+      <c r="A6" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1121,83 +1399,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABE5DF9-E7E6-4E82-9836-F1BB36BDE3D7}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA1E97E-A678-4D10-A8E9-2742BC8C75D4}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
-        <v>26</v>
+      <c r="A1" s="4"/>
+      <c r="B1" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>41</v>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>29</v>
+      <c r="B5" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>30</v>
+      <c r="B6" s="27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>31</v>
+      <c r="B7" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
+      <c r="B8" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1205,73 +1492,173 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABE5DF9-E7E6-4E82-9836-F1BB36BDE3D7}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="1">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="114.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F96EB0-2018-48EE-97B6-0E76930E5B6D}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection sqref="A1:B9"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1279,15 +1666,308 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="B10" s="4"/>
+      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49932A90-361E-4181-8C8F-E4FAF5D597AA}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A5D40A-BA46-49D2-8C19-3C9845DA9A15}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="114.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE81F541-E7EF-4D98-A4E6-EB09412253F2}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B923C15F-39FC-428F-95DF-764CE7F2400E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
About to change to reference each worksheet
This is definitely procrastination now
</commit_message>
<xml_diff>
--- a/Belbin Template.xlsx
+++ b/Belbin Template.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\PersonalityQuestionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C0A91-DC52-4581-9721-3E1CEAF061C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF215A-9B00-4E46-A978-948001E6EBDF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" activeTab="5" xr2:uid="{E0209042-E664-4103-A5FE-D1E5EFD81B12}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" activeTab="7" xr2:uid="{E0209042-E664-4103-A5FE-D1E5EFD81B12}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
-    <sheet name="S1" sheetId="8" r:id="rId2"/>
-    <sheet name="S2" sheetId="4" r:id="rId3"/>
-    <sheet name="S3" sheetId="3" r:id="rId4"/>
-    <sheet name="S4" sheetId="2" r:id="rId5"/>
-    <sheet name="S5" sheetId="5" r:id="rId6"/>
-    <sheet name="S6" sheetId="6" r:id="rId7"/>
-    <sheet name="S7" sheetId="7" r:id="rId8"/>
+    <sheet name="1" sheetId="8" r:id="rId2"/>
+    <sheet name="2" sheetId="4" r:id="rId3"/>
+    <sheet name="3" sheetId="3" r:id="rId4"/>
+    <sheet name="4" sheetId="2" r:id="rId5"/>
+    <sheet name="5" sheetId="5" r:id="rId6"/>
+    <sheet name="6" sheetId="6" r:id="rId7"/>
+    <sheet name="7" sheetId="7" r:id="rId8"/>
     <sheet name="References" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179021"/>
@@ -760,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1B4296-D68F-40AA-A935-AFB247084132}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -934,23 +934,51 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="13"/>
+      <c r="B6" s="23">
+        <f ca="1">VLOOKUP(B$1,INDIRECT(ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="23">
+        <f t="shared" ref="C6:I6" ca="1" si="1">VLOOKUP(C$1,INDIRECT(ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="23">
+        <f ca="1">VLOOKUP(B$1,INDIRECT(ADDRESS(1,1,1,1,$A7)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
+        <v>0</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="7"/>
       <c r="E7" s="11"/>
@@ -958,7 +986,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="13"/>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -966,7 +994,10 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="23">
+        <f ca="1">VLOOKUP(B$1,INDIRECT(ADDRESS(1,1,1,1,$A8)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
+        <v>0</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="7"/>
       <c r="E8" s="11"/>
@@ -974,7 +1005,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="13"/>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1160,35 +1191,35 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <f>C6</f>
+        <f ca="1">C6</f>
         <v>0</v>
       </c>
       <c r="C16">
-        <f>G6</f>
+        <f ca="1">G6</f>
         <v>0</v>
       </c>
       <c r="D16">
-        <f>E6</f>
+        <f ca="1">E6</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f>I6</f>
+        <f ca="1">I6</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>F6</f>
+        <f ca="1">F6</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f>B6</f>
-        <v>0</v>
+        <f ca="1">B6</f>
+        <v>2</v>
       </c>
       <c r="H16">
-        <f>D6</f>
+        <f ca="1">D6</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>H6</f>
+        <f ca="1">H6</f>
         <v>0</v>
       </c>
     </row>
@@ -1209,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <f>B7</f>
+        <f ca="1">B7</f>
         <v>0</v>
       </c>
       <c r="F17">
@@ -1242,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f>B8</f>
+        <f ca="1">B8</f>
         <v>0</v>
       </c>
       <c r="E18">
@@ -1271,36 +1302,48 @@
         <v>9</v>
       </c>
       <c r="B19">
-        <f>SUM(B12:B18)</f>
+        <f ca="1">SUM(B12:B18)</f>
         <v>6</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:I19" si="1">SUM(C12:C18)</f>
+        <f t="shared" ref="C19:I19" ca="1" si="2">SUM(C12:C18)</f>
         <v>4</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>8</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="C22" t="str">
+        <f>ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1)</f>
+        <v>'5'!$A$1:$C$9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="e">
+        <f ca="1">INDIRECT(ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1))</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -1681,13 +1724,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49932A90-361E-4181-8C8F-E4FAF5D597AA}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B9"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1696,21 +1739,24 @@
     <col min="2" max="2" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1718,7 +1764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1726,7 +1772,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
@@ -1734,7 +1780,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
@@ -1742,7 +1788,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -1750,7 +1796,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -1758,7 +1804,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1868,7 +1914,9 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Now uses indirection to fill out results
</commit_message>
<xml_diff>
--- a/Belbin Template.xlsx
+++ b/Belbin Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\PersonalityQuestionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF215A-9B00-4E46-A978-948001E6EBDF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A047D9B1-128C-499E-9ABF-C3BD09B5A7B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" activeTab="7" xr2:uid="{E0209042-E664-4103-A5FE-D1E5EFD81B12}"/>
@@ -286,7 +286,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +316,12 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="ArialMT"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -392,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,6 +445,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,16 +767,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1B4296-D68F-40AA-A935-AFB247084132}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.15" customHeight="1">
@@ -809,30 +825,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="23">
-        <v>1</v>
+        <f t="shared" ref="B2:B5" ca="1" si="0">VLOOKUP(B$1,INDIRECT(ADDRESS(1,1,1,1,$A2)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>2</v>
+        <f t="shared" ref="C2:I8" ca="1" si="1">VLOOKUP(C$1,INDIRECT(ADDRESS(1,1,1,1,$A2)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
+        <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>2</v>
-      </c>
-      <c r="E2" s="11"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
       <c r="F2" s="26">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="G2" s="9">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="H2" s="13">
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="J2">
-        <f>SUM(B2:I2)</f>
-        <v>10</v>
+        <f ca="1">SUM(B2:I2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -840,30 +866,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="23">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D3" s="7">
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="E3" s="11">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="F3" s="26">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="G3" s="9">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="H3" s="13">
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J8" si="0">SUM(B3:I3)</f>
-        <v>10</v>
+        <f t="shared" ref="J3:J8" ca="1" si="2">SUM(B3:I3)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -871,32 +907,40 @@
         <v>3</v>
       </c>
       <c r="B4" s="23">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="D4" s="7">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="E4" s="11">
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="F4" s="26">
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="G4" s="9">
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="H4" s="13">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -904,30 +948,40 @@
         <v>4</v>
       </c>
       <c r="B5" s="23">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D5" s="7">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="E5" s="11">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="F5" s="26">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="G5" s="9">
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="H5" s="13">
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -936,39 +990,39 @@
       </c>
       <c r="B6" s="23">
         <f ca="1">VLOOKUP(B$1,INDIRECT(ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
-        <v>2</v>
-      </c>
-      <c r="C6" s="23">
-        <f t="shared" ref="C6:I6" ca="1" si="1">VLOOKUP(C$1,INDIRECT(ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="23">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" ref="C6:H8" ca="1" si="3">VLOOKUP(C$1,INDIRECT(ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="26">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J6">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -979,14 +1033,36 @@
         <f ca="1">VLOOKUP(B$1,INDIRECT(ADDRESS(1,1,1,1,$A7)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="13"/>
+      <c r="C7" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="26">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J7">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -998,14 +1074,36 @@
         <f ca="1">VLOOKUP(B$1,INDIRECT(ADDRESS(1,1,1,1,$A8)&amp;":"&amp;ADDRESS(9,3,1,1)),3)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="13"/>
+      <c r="C8" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="26">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1043,36 +1141,36 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <f>H2</f>
-        <v>2</v>
+        <f ca="1">H2</f>
+        <v>0</v>
       </c>
       <c r="C12">
-        <f>E2</f>
+        <f ca="1">E2</f>
         <v>0</v>
       </c>
       <c r="D12">
-        <f>G2</f>
-        <v>1</v>
+        <f ca="1">G2</f>
+        <v>0</v>
       </c>
       <c r="E12">
-        <f>D2</f>
-        <v>2</v>
+        <f ca="1">D2</f>
+        <v>0</v>
       </c>
       <c r="F12">
-        <f>B2</f>
-        <v>1</v>
+        <f ca="1">B2</f>
+        <v>0</v>
       </c>
       <c r="G12">
-        <f>I2</f>
-        <v>1</v>
+        <f ca="1">I2</f>
+        <v>0</v>
       </c>
       <c r="H12">
-        <f>C2</f>
-        <v>2</v>
+        <f ca="1">C2</f>
+        <v>0</v>
       </c>
       <c r="I12">
-        <f>F2</f>
-        <v>1</v>
+        <f ca="1">F2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1080,36 +1178,36 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <f>B3</f>
-        <v>2</v>
+        <f ca="1">B3</f>
+        <v>0</v>
       </c>
       <c r="C13">
-        <f>C3</f>
+        <f ca="1">C3</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f>F3</f>
-        <v>1</v>
+        <f ca="1">F3</f>
+        <v>0</v>
       </c>
       <c r="E13">
-        <f>H3</f>
-        <v>3</v>
+        <f ca="1">H3</f>
+        <v>0</v>
       </c>
       <c r="F13">
-        <f>D3</f>
-        <v>3</v>
+        <f ca="1">D3</f>
+        <v>0</v>
       </c>
       <c r="G13">
-        <f>E3</f>
+        <f ca="1">E3</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>G3</f>
+        <f ca="1">G3</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>I3</f>
-        <v>1</v>
+        <f ca="1">I3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1117,35 +1215,35 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <f>I4</f>
-        <v>1</v>
+        <f ca="1">I4</f>
+        <v>0</v>
       </c>
       <c r="C14">
-        <f>B4</f>
-        <v>2</v>
+        <f ca="1">B4</f>
+        <v>0</v>
       </c>
       <c r="D14">
-        <f>D4</f>
+        <f ca="1">D4</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>E4</f>
-        <v>2</v>
+        <f ca="1">E4</f>
+        <v>0</v>
       </c>
       <c r="F14">
-        <f>G4</f>
-        <v>2</v>
+        <f ca="1">G4</f>
+        <v>0</v>
       </c>
       <c r="G14">
-        <f>H4</f>
+        <f ca="1">H4</f>
         <v>0</v>
       </c>
       <c r="H14">
-        <f>F4</f>
-        <v>3</v>
+        <f ca="1">F4</f>
+        <v>0</v>
       </c>
       <c r="I14">
-        <f>C4</f>
+        <f ca="1">C4</f>
         <v>0</v>
       </c>
     </row>
@@ -1154,36 +1252,36 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <f>E5</f>
-        <v>1</v>
+        <f ca="1">E5</f>
+        <v>0</v>
       </c>
       <c r="C15">
-        <f>I5</f>
-        <v>2</v>
+        <f ca="1">I5</f>
+        <v>0</v>
       </c>
       <c r="D15">
-        <f>C5</f>
+        <f ca="1">C5</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>F5</f>
-        <v>1</v>
+        <f ca="1">F5</f>
+        <v>0</v>
       </c>
       <c r="F15">
-        <f>H5</f>
-        <v>1</v>
+        <f ca="1">H5</f>
+        <v>0</v>
       </c>
       <c r="G15">
-        <f>D5</f>
-        <v>1</v>
+        <f ca="1">D5</f>
+        <v>0</v>
       </c>
       <c r="H15">
-        <f>B5</f>
-        <v>1</v>
+        <f ca="1">B5</f>
+        <v>0</v>
       </c>
       <c r="I15">
-        <f>G5</f>
-        <v>3</v>
+        <f ca="1">G5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1212,7 +1310,7 @@
       </c>
       <c r="G16">
         <f ca="1">B6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <f ca="1">D6</f>
@@ -1228,15 +1326,15 @@
         <v>6</v>
       </c>
       <c r="B17">
-        <f>G7</f>
+        <f ca="1">G7</f>
         <v>0</v>
       </c>
       <c r="C17">
-        <f>D7</f>
+        <f ca="1">D7</f>
         <v>0</v>
       </c>
       <c r="D17">
-        <f>H7</f>
+        <f ca="1">H7</f>
         <v>0</v>
       </c>
       <c r="E17">
@@ -1244,19 +1342,19 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <f>I7</f>
+        <f ca="1">I7</f>
         <v>0</v>
       </c>
       <c r="G17">
-        <f>F7</f>
+        <f ca="1">F7</f>
         <v>0</v>
       </c>
       <c r="H17">
-        <f>C7</f>
+        <f ca="1">C7</f>
         <v>0</v>
       </c>
       <c r="I17">
-        <f>E7</f>
+        <f ca="1">E7</f>
         <v>0</v>
       </c>
     </row>
@@ -1265,11 +1363,11 @@
         <v>7</v>
       </c>
       <c r="B18">
-        <f>F8</f>
+        <f ca="1">F8</f>
         <v>0</v>
       </c>
       <c r="C18">
-        <f>H8</f>
+        <f ca="1">H8</f>
         <v>0</v>
       </c>
       <c r="D18">
@@ -1277,23 +1375,23 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <f>G8</f>
+        <f ca="1">G8</f>
         <v>0</v>
       </c>
       <c r="F18">
-        <f>E8</f>
+        <f ca="1">E8</f>
         <v>0</v>
       </c>
       <c r="G18">
-        <f>C8</f>
+        <f ca="1">C8</f>
         <v>0</v>
       </c>
       <c r="H18">
-        <f>I8</f>
+        <f ca="1">I8</f>
         <v>0</v>
       </c>
       <c r="I18">
-        <f>D8</f>
+        <f ca="1">D8</f>
         <v>0</v>
       </c>
     </row>
@@ -1303,47 +1401,35 @@
       </c>
       <c r="B19">
         <f ca="1">SUM(B12:B18)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:I19" ca="1" si="2">SUM(C12:C18)</f>
-        <v>4</v>
+        <f t="shared" ref="C19:I19" ca="1" si="4">SUM(C12:C18)</f>
+        <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="E19">
-        <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="C22" t="str">
-        <f>ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1)</f>
-        <v>'5'!$A$1:$C$9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="e">
-        <f ca="1">INDIRECT(ADDRESS(1,1,1,1,$A6)&amp;":"&amp;ADDRESS(9,3,1,1))</f>
-        <v>#VALUE!</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1353,88 +1439,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0040741-549C-4C0A-B9F2-8D7E11F2B3CC}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C1" sqref="C1:C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="125.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="15" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="25" customFormat="1">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3" s="25" customFormat="1">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" s="25" customFormat="1">
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" s="25" customFormat="1">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1443,90 +1541,102 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA1E97E-A678-4D10-A8E9-2742BC8C75D4}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C1" sqref="C1:D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="112.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="14" spans="1:3">
       <c r="B14" s="3"/>
     </row>
   </sheetData>
@@ -1536,90 +1646,100 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABE5DF9-E7E6-4E82-9836-F1BB36BDE3D7}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
     <sheetView topLeftCell="B1" workbookViewId="1">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C1" sqref="C1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="114.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1628,92 +1748,102 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F96EB0-2018-48EE-97B6-0E76930E5B6D}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C1" sqref="C1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="107.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="B10" s="3"/>
     </row>
   </sheetData>
@@ -1724,13 +1854,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49932A90-361E-4181-8C8F-E4FAF5D597AA}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1739,78 +1869,93 @@
     <col min="2" max="2" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="4"/>
       <c r="B1" s="15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1819,12 +1964,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A5D40A-BA46-49D2-8C19-3C9845DA9A15}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1832,75 +1979,84 @@
     <col min="2" max="2" width="114.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1909,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE81F541-E7EF-4D98-A4E6-EB09412253F2}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C1" sqref="C1:C9"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="B26" sqref="B26"/>
@@ -1924,75 +2080,84 @@
     <col min="2" max="2" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added "Score" header for answer sheets
</commit_message>
<xml_diff>
--- a/Belbin Template.xlsx
+++ b/Belbin Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\PersonalityQuestionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E04C25F-4C29-48B6-BE2A-C6179E71626E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AD67F0-18BD-4D58-90DC-5EBFDB9B7EF8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" activeTab="7" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" activeTab="7" xr2:uid="{E0209042-E664-4103-A5FE-D1E5EFD81B12}"/>
   </bookViews>
   <sheets>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="83">
   <si>
     <t>Section</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>(d)My ability rests in being able to draw people out whenever I detect they have something of value to contribute to group objectives.</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
@@ -776,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1B4296-D68F-40AA-A935-AFB247084132}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
@@ -1449,7 +1452,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C1" sqref="C1:C9"/>
@@ -1467,7 +1470,9 @@
       <c r="B1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:3" s="25" customFormat="1">
       <c r="A2" s="23" t="s">
@@ -1551,7 +1556,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C1" sqref="C1:D9"/>
@@ -1569,7 +1574,9 @@
       <c r="B1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -1656,7 +1663,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
     <sheetView topLeftCell="B1" workbookViewId="1">
       <selection activeCell="C1" sqref="C1:D9"/>
@@ -1674,7 +1681,9 @@
       <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -1758,7 +1767,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C1" sqref="C1:C9"/>
@@ -1776,7 +1785,9 @@
       <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -1864,7 +1875,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C1" sqref="C1:D9"/>
@@ -1882,7 +1893,9 @@
         <v>45</v>
       </c>
       <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="D1" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="23" t="s">
@@ -1974,7 +1987,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C2" sqref="C2"/>
@@ -1991,7 +2004,9 @@
       <c r="B1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -2074,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE81F541-E7EF-4D98-A4E6-EB09412253F2}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="B26" sqref="B26"/>
@@ -2092,7 +2107,9 @@
       <c r="B1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">

</xml_diff>